<commit_message>
water and co reaction added
</commit_message>
<xml_diff>
--- a/RCE/RPMtoDelta.xlsx
+++ b/RCE/RPMtoDelta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexa\Documents\VSCode\Research\PMRModel\RCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBF9778-812F-419D-A1CA-0EBB68C56384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF08B1B-CCBE-494D-8DD2-D51F4F38C2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{5C0E03CF-3BAB-4377-A482-84AC69AF0267}"/>
   </bookViews>
@@ -3934,8 +3934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B24714F3-5E9E-4775-9E72-958E1772AAEE}">
   <dimension ref="B2:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>